<commit_message>
- approved and printed final manuscript for book binding - project success | May 2022 |
</commit_message>
<xml_diff>
--- a/Main papers/Data_Log.xlsx
+++ b/Main papers/Data_Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engr. Irvin Gil Files\Documents\4th year 1st sem\Thesis 1 and 2\Main papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEC325A-24BA-4585-B736-30EABFEDED73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85AB5EA-D71A-4D15-AE6C-D6AFAE14ED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12504" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorted data" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,12 @@
     <sheet name="Schedule project" sheetId="5" r:id="rId3"/>
     <sheet name="Statistical result" sheetId="4" r:id="rId4"/>
     <sheet name="Meter unit accuracy test" sheetId="3" r:id="rId5"/>
+    <sheet name="sample" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="176">
   <si>
     <t>Date</t>
   </si>
@@ -201,9 +203,6 @@
     <t>Voltage</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
     <t>Trial 1</t>
   </si>
   <si>
@@ -418,6 +417,159 @@
   </si>
   <si>
     <t>Week 4</t>
+  </si>
+  <si>
+    <t>4/24/2022</t>
+  </si>
+  <si>
+    <t>4/25/2022</t>
+  </si>
+  <si>
+    <t>4/26/2022</t>
+  </si>
+  <si>
+    <t>4/27/2022</t>
+  </si>
+  <si>
+    <t>4/28/2022</t>
+  </si>
+  <si>
+    <t>5373_4/24/2022_22:0_0.000</t>
+  </si>
+  <si>
+    <t>2923_4/25/2022_5:39_0.000</t>
+  </si>
+  <si>
+    <t>2923_4/25/2022_6:4_0.056</t>
+  </si>
+  <si>
+    <t>2267_4/25/2022_7:59_0.338</t>
+  </si>
+  <si>
+    <t>5373_4/25/2022_11:52_0.495</t>
+  </si>
+  <si>
+    <t>0007_4/25/2022_19:40_0.000</t>
+  </si>
+  <si>
+    <t>2923_4/25/2022_19:44_0.000</t>
+  </si>
+  <si>
+    <t>8866_4/25/2022_20:5_0.000</t>
+  </si>
+  <si>
+    <t>2267_4/25/2022_20:23_0.000</t>
+  </si>
+  <si>
+    <t>4900_4/25/2022_22:39_0.000</t>
+  </si>
+  <si>
+    <t>5906_4/26/2022_5:25_0.000</t>
+  </si>
+  <si>
+    <t>2923_4/26/2022_6:15_0.497</t>
+  </si>
+  <si>
+    <t>2267_4/26/2022_6:49_0.115</t>
+  </si>
+  <si>
+    <t>2923_4/26/2022_11:10_0.000</t>
+  </si>
+  <si>
+    <t>9644_4/26/2022_17:3_0.001</t>
+  </si>
+  <si>
+    <t>9644_4/26/2022_17:14_0.001</t>
+  </si>
+  <si>
+    <t>0007_4/26/2022_17:54_0.000</t>
+  </si>
+  <si>
+    <t>0007_4/26/2022_17:56_0.000</t>
+  </si>
+  <si>
+    <t>9644_4/26/2022_17:57_0.000</t>
+  </si>
+  <si>
+    <t>5373_4/26/2022_17:59_0.000</t>
+  </si>
+  <si>
+    <t>0007_4/26/2022_18:0_0.000</t>
+  </si>
+  <si>
+    <t>9644_4/26/2022_18:33_0.207</t>
+  </si>
+  <si>
+    <t>2923_4/27/2022_6:37_0.015</t>
+  </si>
+  <si>
+    <t>2267_4/27/2022_6:44_0.070</t>
+  </si>
+  <si>
+    <t>9880_4/27/2022_9:45_0.199</t>
+  </si>
+  <si>
+    <t>2923_4/27/2022_13:53_0.045</t>
+  </si>
+  <si>
+    <t>5906_4/27/2022_17:3_0.039</t>
+  </si>
+  <si>
+    <t>5373_4/27/2022_17:38_0.284</t>
+  </si>
+  <si>
+    <t>2267_4/27/2022_17:41_0.000</t>
+  </si>
+  <si>
+    <t>5906_4/27/2022_18:9_0.193</t>
+  </si>
+  <si>
+    <t>2267_4/27/2022_22:13_0.098</t>
+  </si>
+  <si>
+    <t>0007_4/28/2022_9:8_0.000</t>
+  </si>
+  <si>
+    <t>Consumption</t>
+  </si>
+  <si>
+    <t>Sum of Consumption</t>
+  </si>
+  <si>
+    <t>10 pm</t>
+  </si>
+  <si>
+    <t>5 am</t>
+  </si>
+  <si>
+    <t>6 am</t>
+  </si>
+  <si>
+    <t>7 am</t>
+  </si>
+  <si>
+    <t>11 am</t>
+  </si>
+  <si>
+    <t>7 pm</t>
+  </si>
+  <si>
+    <t>8 pm</t>
+  </si>
+  <si>
+    <t>5 pm</t>
+  </si>
+  <si>
+    <t>6 pm</t>
+  </si>
+  <si>
+    <t>9 am</t>
+  </si>
+  <si>
+    <t>1 pm</t>
+  </si>
+  <si>
+    <t>Current (Amp)</t>
   </si>
 </sst>
 </file>
@@ -428,7 +580,7 @@
     <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +597,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -633,23 +792,25 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1890,6 +2051,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>17929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>936384</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>90485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F432DC0-BDF5-1C9E-B64A-052BFB09AF89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7566212" y="3164541"/>
+          <a:ext cx="2953443" cy="969026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Benjie Basa" refreshedDate="44679.902136689816" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20" xr:uid="{00000000-000A-0000-FFFF-FFFF06000000}">
   <cacheSource type="worksheet">
@@ -2056,6 +2266,184 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Engr. Irvin Gil" refreshedDate="44684.74999074074" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="33" xr:uid="{358BF366-020F-4409-B960-29705D28DF6C}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E1:I34" sheet="sample"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Passcode" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="7" maxValue="9880"/>
+    </cacheField>
+    <cacheField name="Date" numFmtId="0">
+      <sharedItems count="5">
+        <s v="4/24/2022"/>
+        <s v="4/25/2022"/>
+        <s v="4/26/2022"/>
+        <s v="4/27/2022"/>
+        <s v="4/28/2022"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Time" numFmtId="20">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="1899-12-30T05:25:00" maxDate="1899-12-30T22:39:00" count="31">
+        <d v="1899-12-30T22:00:00"/>
+        <d v="1899-12-30T05:39:00"/>
+        <d v="1899-12-30T06:04:00"/>
+        <d v="1899-12-30T07:59:00"/>
+        <d v="1899-12-30T11:52:00"/>
+        <d v="1899-12-30T19:40:00"/>
+        <d v="1899-12-30T19:44:00"/>
+        <d v="1899-12-30T20:05:00"/>
+        <d v="1899-12-30T20:23:00"/>
+        <d v="1899-12-30T22:39:00"/>
+        <d v="1899-12-30T05:25:00"/>
+        <d v="1899-12-30T06:15:00"/>
+        <d v="1899-12-30T06:49:00"/>
+        <d v="1899-12-30T11:10:00"/>
+        <d v="1899-12-30T17:03:00"/>
+        <d v="1899-12-30T17:14:00"/>
+        <d v="1899-12-30T17:54:00"/>
+        <d v="1899-12-30T17:56:00"/>
+        <d v="1899-12-30T17:57:00"/>
+        <d v="1899-12-30T17:59:00"/>
+        <d v="1899-12-30T18:00:00"/>
+        <d v="1899-12-30T18:33:00"/>
+        <d v="1899-12-30T06:37:00"/>
+        <d v="1899-12-30T06:44:00"/>
+        <d v="1899-12-30T09:45:00"/>
+        <d v="1899-12-30T13:53:00"/>
+        <d v="1899-12-30T17:38:00"/>
+        <d v="1899-12-30T17:41:00"/>
+        <d v="1899-12-30T18:09:00"/>
+        <d v="1899-12-30T22:13:00"/>
+        <d v="1899-12-30T09:08:00"/>
+      </sharedItems>
+      <fieldGroup par="5" base="2">
+        <rangePr groupBy="minutes" startDate="1899-12-30T05:25:00" endDate="1899-12-30T22:39:00"/>
+        <groupItems count="62">
+          <s v="&lt;00/01/1900"/>
+          <s v=":00"/>
+          <s v=":01"/>
+          <s v=":02"/>
+          <s v=":03"/>
+          <s v=":04"/>
+          <s v=":05"/>
+          <s v=":06"/>
+          <s v=":07"/>
+          <s v=":08"/>
+          <s v=":09"/>
+          <s v=":10"/>
+          <s v=":11"/>
+          <s v=":12"/>
+          <s v=":13"/>
+          <s v=":14"/>
+          <s v=":15"/>
+          <s v=":16"/>
+          <s v=":17"/>
+          <s v=":18"/>
+          <s v=":19"/>
+          <s v=":20"/>
+          <s v=":21"/>
+          <s v=":22"/>
+          <s v=":23"/>
+          <s v=":24"/>
+          <s v=":25"/>
+          <s v=":26"/>
+          <s v=":27"/>
+          <s v=":28"/>
+          <s v=":29"/>
+          <s v=":30"/>
+          <s v=":31"/>
+          <s v=":32"/>
+          <s v=":33"/>
+          <s v=":34"/>
+          <s v=":35"/>
+          <s v=":36"/>
+          <s v=":37"/>
+          <s v=":38"/>
+          <s v=":39"/>
+          <s v=":40"/>
+          <s v=":41"/>
+          <s v=":42"/>
+          <s v=":43"/>
+          <s v=":44"/>
+          <s v=":45"/>
+          <s v=":46"/>
+          <s v=":47"/>
+          <s v=":48"/>
+          <s v=":49"/>
+          <s v=":50"/>
+          <s v=":51"/>
+          <s v=":52"/>
+          <s v=":53"/>
+          <s v=":54"/>
+          <s v=":55"/>
+          <s v=":56"/>
+          <s v=":57"/>
+          <s v=":58"/>
+          <s v=":59"/>
+          <s v="&gt;00/01/1900"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+    <cacheField name="Consumption" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.497"/>
+    </cacheField>
+    <cacheField name="User" numFmtId="0">
+      <sharedItems count="9">
+        <s v="Benjie Basa"/>
+        <s v="Irvin Gil Mercado"/>
+        <s v="Lyndon Diacosta"/>
+        <s v="Renante Mayor"/>
+        <s v="Runnel Jay Barcelon"/>
+        <s v="John Lerie Cadarve"/>
+        <s v="Solomon Lim"/>
+        <s v="Mark Neil Crisostomo"/>
+        <s v="John Melvin Caday"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Hours" numFmtId="0" databaseField="0">
+      <fieldGroup base="2">
+        <rangePr groupBy="hours" startDate="1899-12-30T05:25:00" endDate="1899-12-30T22:39:00"/>
+        <groupItems count="26">
+          <s v="&lt;00/01/1900"/>
+          <s v="12 am"/>
+          <s v="1 am"/>
+          <s v="2 am"/>
+          <s v="3 am"/>
+          <s v="4 am"/>
+          <s v="5 am"/>
+          <s v="6 am"/>
+          <s v="7 am"/>
+          <s v="8 am"/>
+          <s v="9 am"/>
+          <s v="10 am"/>
+          <s v="11 am"/>
+          <s v="12 pm"/>
+          <s v="1 pm"/>
+          <s v="2 pm"/>
+          <s v="3 pm"/>
+          <s v="4 pm"/>
+          <s v="5 pm"/>
+          <s v="6 pm"/>
+          <s v="7 pm"/>
+          <s v="8 pm"/>
+          <s v="9 pm"/>
+          <s v="10 pm"/>
+          <s v="11 pm"/>
+          <s v="&gt;00/01/1900"/>
+        </groupItems>
+      </fieldGroup>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="20">
   <r>
@@ -2197,6 +2585,242 @@
     <x v="19"/>
     <n v="0.05"/>
     <x v="8"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="33">
+  <r>
+    <n v="5373"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="5.6000000000000001E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2267"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="0.33800000000000002"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5373"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="0.495"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="8866"/>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="2267"/>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="4900"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="5906"/>
+    <x v="2"/>
+    <x v="10"/>
+    <n v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="2"/>
+    <x v="11"/>
+    <n v="0.497"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2267"/>
+    <x v="2"/>
+    <x v="12"/>
+    <n v="0.115"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="2"/>
+    <x v="13"/>
+    <n v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="9644"/>
+    <x v="2"/>
+    <x v="14"/>
+    <n v="1E-3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="9644"/>
+    <x v="2"/>
+    <x v="15"/>
+    <n v="1E-3"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="2"/>
+    <x v="16"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="2"/>
+    <x v="17"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="9644"/>
+    <x v="2"/>
+    <x v="18"/>
+    <n v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="5373"/>
+    <x v="2"/>
+    <x v="19"/>
+    <n v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="2"/>
+    <x v="20"/>
+    <n v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="9644"/>
+    <x v="2"/>
+    <x v="21"/>
+    <n v="0.20699999999999999"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="3"/>
+    <x v="22"/>
+    <n v="1.4999999999999999E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2267"/>
+    <x v="3"/>
+    <x v="23"/>
+    <n v="7.0000000000000007E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="9880"/>
+    <x v="3"/>
+    <x v="24"/>
+    <n v="0.19900000000000001"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="2923"/>
+    <x v="3"/>
+    <x v="25"/>
+    <n v="4.4999999999999998E-2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="5906"/>
+    <x v="3"/>
+    <x v="14"/>
+    <n v="3.9E-2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="5373"/>
+    <x v="3"/>
+    <x v="26"/>
+    <n v="0.28399999999999997"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2267"/>
+    <x v="3"/>
+    <x v="27"/>
+    <n v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="5906"/>
+    <x v="3"/>
+    <x v="28"/>
+    <n v="0.193"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="2267"/>
+    <x v="3"/>
+    <x v="29"/>
+    <n v="9.8000000000000004E-2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="4"/>
+    <x v="30"/>
+    <n v="0"/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2517,6 +3141,270 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{29B98756-BD55-4E4B-A481-8001D17D59D5}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M1:W28" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="20" showAll="0">
+      <items count="63">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="5"/>
+        <item x="8"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="27">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="14"/>
+        <item sd="0" x="15"/>
+        <item sd="0" x="16"/>
+        <item sd="0" x="17"/>
+        <item sd="0" x="18"/>
+        <item sd="0" x="19"/>
+        <item sd="0" x="20"/>
+        <item sd="0" x="21"/>
+        <item sd="0" x="22"/>
+        <item sd="0" x="23"/>
+        <item sd="0" x="24"/>
+        <item sd="0" x="25"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="1"/>
+    <field x="5"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="26">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Consumption" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2783,7 +3671,7 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4532,7 +5420,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4561,10 +5449,10 @@
         <v>50</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>101</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>102</v>
       </c>
       <c r="E2" s="18"/>
     </row>
@@ -4584,7 +5472,7 @@
       <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="34">
+      <c r="A4" s="39">
         <v>44677</v>
       </c>
       <c r="B4" s="14">
@@ -4598,7 +5486,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="14">
         <v>3</v>
       </c>
@@ -4610,7 +5498,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="34"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="14">
         <v>4</v>
       </c>
@@ -4622,7 +5510,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="14">
         <v>5</v>
       </c>
@@ -4634,7 +5522,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="34"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="14">
         <v>6</v>
       </c>
@@ -4647,7 +5535,7 @@
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="34"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="14">
         <v>7</v>
       </c>
@@ -4660,7 +5548,7 @@
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="14">
         <v>8</v>
       </c>
@@ -4673,7 +5561,7 @@
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="34">
+      <c r="A11" s="39">
         <v>44678</v>
       </c>
       <c r="B11" s="14">
@@ -4688,7 +5576,7 @@
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="14">
         <v>10</v>
       </c>
@@ -4701,7 +5589,7 @@
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="14">
         <v>11</v>
       </c>
@@ -4714,7 +5602,7 @@
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="14">
         <v>12</v>
       </c>
@@ -4727,7 +5615,7 @@
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="14">
         <v>13</v>
       </c>
@@ -4739,7 +5627,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="14">
         <v>14</v>
       </c>
@@ -4752,7 +5640,7 @@
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="14">
         <v>15</v>
       </c>
@@ -4765,7 +5653,7 @@
       <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="34"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="14">
         <v>16</v>
       </c>
@@ -4778,7 +5666,7 @@
       <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="34">
+      <c r="A19" s="39">
         <v>44679</v>
       </c>
       <c r="B19" s="14">
@@ -4793,7 +5681,7 @@
       <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="34"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="14">
         <v>18</v>
       </c>
@@ -4806,7 +5694,7 @@
       <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="34"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="14">
         <v>19</v>
       </c>
@@ -4879,7 +5767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCBA49B-02A1-4446-AA96-491F6B07596C}">
   <dimension ref="A4:AK14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:AK14"/>
     </sheetView>
   </sheetViews>
@@ -4890,189 +5778,189 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35" t="s">
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35" t="s">
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35" t="s">
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35" t="s">
+      <c r="W4" s="40"/>
+      <c r="X4" s="40"/>
+      <c r="Y4" s="40"/>
+      <c r="Z4" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35" t="s">
+      <c r="AA4" s="40"/>
+      <c r="AB4" s="40"/>
+      <c r="AC4" s="40"/>
+      <c r="AD4" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35" t="s">
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="35"/>
-      <c r="AG4" s="35"/>
-      <c r="AH4" s="35" t="s">
+      <c r="AI4" s="40"/>
+      <c r="AJ4" s="40"/>
+      <c r="AK4" s="40"/>
+    </row>
+    <row r="5" spans="1:37" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
+      <c r="B5" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="AI4" s="35"/>
-      <c r="AJ4" s="35"/>
-      <c r="AK4" s="35"/>
-    </row>
-    <row r="5" spans="1:37" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="38" t="s">
+      <c r="C5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="E5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="H5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="I5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="38" t="s">
+      <c r="J5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="K5" s="38" t="s">
+      <c r="L5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="L5" s="38" t="s">
+      <c r="M5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="M5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="O5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="O5" s="38" t="s">
+      <c r="P5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="P5" s="38" t="s">
+      <c r="Q5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="Q5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="R5" s="38" t="s">
+      <c r="R5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="S5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="T5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="T5" s="38" t="s">
+      <c r="U5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="U5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="V5" s="38" t="s">
+      <c r="V5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="W5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="W5" s="38" t="s">
+      <c r="X5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="X5" s="38" t="s">
+      <c r="Y5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="Y5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z5" s="38" t="s">
+      <c r="Z5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="AA5" s="38" t="s">
+      <c r="AB5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="AB5" s="38" t="s">
+      <c r="AC5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="AC5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD5" s="38" t="s">
+      <c r="AD5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="AE5" s="38" t="s">
+      <c r="AF5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="AF5" s="38" t="s">
+      <c r="AG5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="AG5" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="AH5" s="38" t="s">
+      <c r="AH5" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI5" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="AI5" s="38" t="s">
+      <c r="AJ5" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="AJ5" s="38" t="s">
+      <c r="AK5" s="34" t="s">
         <v>124</v>
-      </c>
-      <c r="AK5" s="38" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
+        <v>103</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
       <c r="L6" s="25"/>
       <c r="M6" s="25"/>
       <c r="N6" s="25"/>
@@ -5102,7 +5990,7 @@
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -5113,11 +6001,11 @@
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
       <c r="R7" s="25"/>
@@ -5129,13 +6017,13 @@
       <c r="X7" s="25"/>
       <c r="Y7" s="25"/>
       <c r="Z7" s="25"/>
-      <c r="AA7" s="39"/>
-      <c r="AB7" s="39"/>
-      <c r="AC7" s="39"/>
-      <c r="AD7" s="39"/>
-      <c r="AE7" s="39"/>
-      <c r="AF7" s="39"/>
-      <c r="AG7" s="39"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="35"/>
+      <c r="AD7" s="35"/>
+      <c r="AE7" s="35"/>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="35"/>
       <c r="AH7" s="25"/>
       <c r="AI7" s="25"/>
       <c r="AJ7" s="25"/>
@@ -5143,7 +6031,7 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -5156,18 +6044,18 @@
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="40"/>
-      <c r="X8" s="40"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
       <c r="Y8" s="25"/>
       <c r="Z8" s="25"/>
       <c r="AA8" s="25"/>
@@ -5184,7 +6072,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -5193,31 +6081,31 @@
       <c r="F9" s="25"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="40"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="36"/>
       <c r="Y9" s="25"/>
-      <c r="Z9" s="39"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="39"/>
-      <c r="AC9" s="39"/>
-      <c r="AD9" s="39"/>
-      <c r="AE9" s="39"/>
-      <c r="AF9" s="39"/>
-      <c r="AG9" s="39"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="35"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35"/>
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
       <c r="AH9" s="25"/>
       <c r="AI9" s="25"/>
       <c r="AJ9" s="25"/>
@@ -5225,7 +6113,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -5241,24 +6129,24 @@
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
       <c r="O10" s="25"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
       <c r="U10" s="25"/>
       <c r="V10" s="25"/>
       <c r="W10" s="25"/>
       <c r="X10" s="25"/>
       <c r="Y10" s="25"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="39"/>
-      <c r="AG10" s="39"/>
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="35"/>
+      <c r="AC10" s="35"/>
+      <c r="AD10" s="35"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="35"/>
       <c r="AH10" s="25"/>
       <c r="AI10" s="25"/>
       <c r="AJ10" s="25"/>
@@ -5266,7 +6154,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -5292,14 +6180,14 @@
       <c r="W11" s="25"/>
       <c r="X11" s="25"/>
       <c r="Y11" s="25"/>
-      <c r="Z11" s="39"/>
-      <c r="AA11" s="39"/>
-      <c r="AB11" s="39"/>
-      <c r="AC11" s="39"/>
-      <c r="AD11" s="39"/>
-      <c r="AE11" s="39"/>
-      <c r="AF11" s="39"/>
-      <c r="AG11" s="39"/>
+      <c r="Z11" s="35"/>
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="35"/>
+      <c r="AC11" s="35"/>
+      <c r="AD11" s="35"/>
+      <c r="AE11" s="35"/>
+      <c r="AF11" s="35"/>
+      <c r="AG11" s="35"/>
       <c r="AH11" s="25"/>
       <c r="AI11" s="25"/>
       <c r="AJ11" s="25"/>
@@ -5307,7 +6195,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -5333,22 +6221,22 @@
       <c r="W12" s="25"/>
       <c r="X12" s="25"/>
       <c r="Y12" s="25"/>
-      <c r="Z12" s="39"/>
-      <c r="AA12" s="39"/>
-      <c r="AB12" s="39"/>
-      <c r="AC12" s="39"/>
-      <c r="AD12" s="39"/>
-      <c r="AE12" s="39"/>
-      <c r="AF12" s="39"/>
-      <c r="AG12" s="39"/>
-      <c r="AH12" s="39"/>
-      <c r="AI12" s="39"/>
-      <c r="AJ12" s="40"/>
+      <c r="Z12" s="35"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="35"/>
+      <c r="AD12" s="35"/>
+      <c r="AE12" s="35"/>
+      <c r="AF12" s="35"/>
+      <c r="AG12" s="35"/>
+      <c r="AH12" s="35"/>
+      <c r="AI12" s="35"/>
+      <c r="AJ12" s="36"/>
       <c r="AK12" s="25"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -5383,13 +6271,13 @@
       <c r="AF13" s="25"/>
       <c r="AG13" s="25"/>
       <c r="AH13" s="25"/>
-      <c r="AI13" s="39"/>
-      <c r="AJ13" s="39"/>
+      <c r="AI13" s="35"/>
+      <c r="AJ13" s="35"/>
       <c r="AK13" s="25"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -5425,8 +6313,8 @@
       <c r="AG14" s="25"/>
       <c r="AH14" s="25"/>
       <c r="AI14" s="25"/>
-      <c r="AJ14" s="39"/>
-      <c r="AK14" s="39"/>
+      <c r="AJ14" s="35"/>
+      <c r="AK14" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5465,82 +6353,82 @@
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L10" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" t="s">
         <v>79</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>80</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>81</v>
-      </c>
-      <c r="O10" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" t="s">
         <v>93</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>95</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>96</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>97</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>98</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>99</v>
       </c>
-      <c r="H11" t="s">
-        <v>100</v>
-      </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L11">
         <v>5</v>
@@ -5578,7 +6466,7 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L12">
         <v>10</v>
@@ -5610,7 +6498,7 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L13">
         <v>10</v>
@@ -5642,7 +6530,7 @@
         <v>4</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L14">
         <v>4</v>
@@ -5680,7 +6568,7 @@
         <v>4</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L15">
         <v>6</v>
@@ -5715,7 +6603,7 @@
         <v>4</v>
       </c>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L16">
         <v>10</v>
@@ -5747,7 +6635,7 @@
         <v>4</v>
       </c>
       <c r="K17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L17">
         <v>10</v>
@@ -5859,7 +6747,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22">
         <f>AVERAGE(B12:B21)</f>
@@ -5896,33 +6784,33 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -5948,7 +6836,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -5962,7 +6850,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -5973,7 +6861,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -5987,19 +6875,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E2C038-E8F0-4FD0-A91B-CDDE2AD167C4}">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:N14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="16.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.3">
@@ -6009,20 +6895,20 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="23"/>
-      <c r="B3" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="35"/>
+      <c r="B3" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="40"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -6033,13 +6919,13 @@
         <v>52</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="E4" t="s">
         <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
@@ -6063,7 +6949,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="25">
         <v>235</v>
@@ -6074,33 +6960,33 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="26">
         <f>ABS(((B5-B6)/B6)*100)</f>
         <v>8.5106382978718573E-2</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="36"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="V7" s="42"/>
     </row>
     <row r="8" spans="1:22" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L8" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M8" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="29" t="s">
         <v>67</v>
-      </c>
-      <c r="N8" s="29" t="s">
-        <v>68</v>
       </c>
       <c r="O8" s="28"/>
       <c r="P8" s="28"/>
@@ -6111,7 +6997,7 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -6122,7 +7008,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="22"/>
       <c r="L9" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M9" s="31">
         <v>8.4902131380768742E-2</v>
@@ -6133,24 +7019,24 @@
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
-      <c r="B10" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35" t="s">
+      <c r="B10" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I10" s="35"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="40"/>
       <c r="L10" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M10" s="31">
         <v>0.14323068562115215</v>
@@ -6165,28 +7051,28 @@
         <v>52</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="F11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="H11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M11" s="31">
         <v>9.8816655246554322E-2</v>
@@ -6220,7 +7106,7 @@
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="L12" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M12" s="31">
         <v>0.11389442582040943</v>
@@ -6231,7 +7117,7 @@
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="25">
         <v>235.4</v>
@@ -6254,7 +7140,7 @@
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
       <c r="L13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M13" s="31">
         <v>9.856581633147958E-2</v>
@@ -6265,7 +7151,7 @@
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="26">
         <f t="shared" ref="B14:G14" si="0">ABS(((B12-B13)/B13)*100)</f>
@@ -6300,7 +7186,7 @@
         <v>0.4489949168946426</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M14" s="31">
         <f>AVERAGE(M9:M13)</f>
@@ -6313,7 +7199,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -6326,22 +7212,22 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
-      <c r="B17" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35" t="s">
+      <c r="B17" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="35"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="40"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
@@ -6349,25 +7235,25 @@
         <v>52</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>52</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>52</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="H18" s="25" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -6397,7 +7283,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="25">
         <v>237.6</v>
@@ -6422,7 +7308,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="26">
         <f t="shared" ref="B21:G21" si="1">ABS(((B19-B20)/B20)*100)</f>
@@ -6459,7 +7345,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -6472,22 +7358,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
-      <c r="B24" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35" t="s">
+      <c r="B24" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" s="35"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I24" s="40"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
@@ -6495,25 +7381,25 @@
         <v>52</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>52</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="F25" s="25" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="H25" s="25" t="s">
         <v>52</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -6543,7 +7429,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="25">
         <v>236.9</v>
@@ -6568,7 +7454,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="26">
         <f t="shared" ref="B28:G28" si="2">ABS(((B26-B27)/B27)*100)</f>
@@ -6605,7 +7491,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -6618,22 +7504,22 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
-      <c r="B31" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35" t="s">
+      <c r="B31" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I31" s="35"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="40"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
@@ -6641,25 +7527,25 @@
         <v>52</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>52</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="F32" s="25" t="s">
         <v>52</v>
       </c>
       <c r="G32" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="H32" s="25" t="s">
         <v>52</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -6689,7 +7575,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="25">
         <v>237.2</v>
@@ -6714,7 +7600,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="26">
         <f t="shared" ref="B35:G35" si="3">ABS(((B33-B34)/B34)*100)</f>
@@ -6751,7 +7637,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -6764,22 +7650,22 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
-      <c r="B38" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35" t="s">
+      <c r="B38" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="I38" s="35"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" s="40"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
@@ -6787,25 +7673,25 @@
         <v>52</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>52</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>52</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
       <c r="H39" s="25" t="s">
         <v>52</v>
       </c>
       <c r="I39" s="25" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -6835,7 +7721,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="25">
         <v>236.9</v>
@@ -6860,7 +7746,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B42" s="26">
         <f t="shared" ref="B42:G42" si="4">ABS(((B40-B41)/B41)*100)</f>
@@ -6897,6 +7783,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="S7:T7"/>
     <mergeCell ref="U7:V7"/>
@@ -6913,18 +7809,1410 @@
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9516D0F7-EDF5-408F-ACA4-55E449EE5C07}">
+  <dimension ref="A1:W44"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="E2">
+        <v>5373</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="str">
+        <f>VLOOKUP(E2,$A$35:$B$44,2,FALSE)</f>
+        <v>Benjie Basa</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="E3">
+        <v>2923</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.23541666666666669</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I34" si="0">VLOOKUP(E3,$A$35:$B$44,2,FALSE)</f>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="E4">
+        <v>2923</v>
+      </c>
+      <c r="F4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.23541666666666669</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="E5">
+        <v>2923</v>
+      </c>
+      <c r="F5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="H5">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0.495</v>
+      </c>
+      <c r="O5" s="6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
+        <v>0</v>
+      </c>
+      <c r="U5" s="6">
+        <v>0</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6">
+        <v>0.88900000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="E6">
+        <v>2267</v>
+      </c>
+      <c r="F6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="H6">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon Diacosta</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="E7">
+        <v>5373</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.49444444444444446</v>
+      </c>
+      <c r="H7">
+        <v>0.495</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>Benjie Basa</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>Renante Mayor</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9">
+        <v>2923</v>
+      </c>
+      <c r="F9" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.8222222222222223</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0.495</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="E10">
+        <v>8866</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.83680555555555547</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>Runnel Jay Barcelon</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6">
+        <v>0</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="E11">
+        <v>2267</v>
+      </c>
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon Diacosta</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6">
+        <v>0</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6">
+        <v>0</v>
+      </c>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="E12">
+        <v>4900</v>
+      </c>
+      <c r="F12" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.94374999999999998</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>John Lerie Cadarve</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="E13">
+        <v>5906</v>
+      </c>
+      <c r="F13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.22569444444444445</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>Solomon Lim</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0.497</v>
+      </c>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6">
+        <v>0.115</v>
+      </c>
+      <c r="S13" s="6">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="T13" s="6">
+        <v>0</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6">
+        <v>0</v>
+      </c>
+      <c r="W13" s="6">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="E14">
+        <v>2923</v>
+      </c>
+      <c r="F14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="H14">
+        <v>0.497</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6">
+        <v>0</v>
+      </c>
+      <c r="W14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="E15">
+        <v>2267</v>
+      </c>
+      <c r="F15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.28402777777777777</v>
+      </c>
+      <c r="H15">
+        <v>0.115</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon Diacosta</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6">
+        <v>0.497</v>
+      </c>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6">
+        <v>0.115</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6">
+        <v>0.61199999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="E16">
+        <v>2923</v>
+      </c>
+      <c r="F16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="E17">
+        <v>9644</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.7104166666666667</v>
+      </c>
+      <c r="H17">
+        <v>1E-3</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Neil Crisostomo</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="N17" s="6">
+        <v>0</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="T17" s="6">
+        <v>0</v>
+      </c>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="E18">
+        <v>9644</v>
+      </c>
+      <c r="F18" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.71805555555555556</v>
+      </c>
+      <c r="H18">
+        <v>1E-3</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Neil Crisostomo</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="T18" s="6">
+        <v>0</v>
+      </c>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.74583333333333324</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>Renante Mayor</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="O19" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="R19" s="6">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="W19" s="6">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.74722222222222223</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>Renante Mayor</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6"/>
+      <c r="W20" s="6">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="E21">
+        <v>9644</v>
+      </c>
+      <c r="F21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.74791666666666667</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Neil Crisostomo</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6">
+        <v>0.19900000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="E22">
+        <v>5373</v>
+      </c>
+      <c r="F22" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.74930555555555556</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>Benjie Basa</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6"/>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6"/>
+      <c r="W22" s="6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="E23">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>Renante Mayor</v>
+      </c>
+      <c r="M23" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="N23" s="6">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6">
+        <v>0</v>
+      </c>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="W23" s="6">
+        <v>0.32299999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="E24">
+        <v>9644</v>
+      </c>
+      <c r="F24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.7729166666666667</v>
+      </c>
+      <c r="H24">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="0"/>
+        <v>Mark Neil Crisostomo</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6">
+        <v>0.193</v>
+      </c>
+      <c r="W24" s="6">
+        <v>0.193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="E25">
+        <v>2923</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.27569444444444446</v>
+      </c>
+      <c r="H25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="E26">
+        <v>2267</v>
+      </c>
+      <c r="F26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.28055555555555556</v>
+      </c>
+      <c r="H26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon Diacosta</v>
+      </c>
+      <c r="M26" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6">
+        <v>0</v>
+      </c>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="E27">
+        <v>9880</v>
+      </c>
+      <c r="F27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="H27">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="0"/>
+        <v>John Melvin Caday</v>
+      </c>
+      <c r="M27" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6">
+        <v>0</v>
+      </c>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="E28">
+        <v>2923</v>
+      </c>
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.57847222222222217</v>
+      </c>
+      <c r="H28">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="0"/>
+        <v>Irvin Gil Mercado</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0.77899999999999991</v>
+      </c>
+      <c r="O28" s="6">
+        <v>0.6130000000000001</v>
+      </c>
+      <c r="P28" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="6">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="R28" s="6">
+        <v>0.621</v>
+      </c>
+      <c r="S28" s="6">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="T28" s="6">
+        <v>0</v>
+      </c>
+      <c r="U28" s="6">
+        <v>0</v>
+      </c>
+      <c r="V28" s="6">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="W28" s="6">
+        <v>2.653</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="E29">
+        <v>5906</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.7104166666666667</v>
+      </c>
+      <c r="H29">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="0"/>
+        <v>Solomon Lim</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="E30">
+        <v>5373</v>
+      </c>
+      <c r="F30" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.73472222222222217</v>
+      </c>
+      <c r="H30">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="0"/>
+        <v>Benjie Basa</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="E31">
+        <v>2267</v>
+      </c>
+      <c r="F31" t="s">
+        <v>128</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon Diacosta</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="E32">
+        <v>5906</v>
+      </c>
+      <c r="F32" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="H32">
+        <v>0.193</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="0"/>
+        <v>Solomon Lim</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="E33">
+        <v>2267</v>
+      </c>
+      <c r="F33" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.92569444444444438</v>
+      </c>
+      <c r="H33">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="0"/>
+        <v>Lyndon Diacosta</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="0"/>
+        <v>Renante Mayor</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="38">
+        <v>2923</v>
+      </c>
+      <c r="B35" s="37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="38">
+        <v>5373</v>
+      </c>
+      <c r="B36" s="37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="38">
+        <v>7</v>
+      </c>
+      <c r="B37" s="37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="38">
+        <v>9644</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="38">
+        <v>2267</v>
+      </c>
+      <c r="B39" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="38">
+        <v>5906</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="38">
+        <v>553</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="38">
+        <v>4900</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="38">
+        <v>9880</v>
+      </c>
+      <c r="B43" s="37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="38">
+        <v>8866</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>